<commit_message>
Add second page of use cases for Registration.
</commit_message>
<xml_diff>
--- a/Use Cases.xlsx
+++ b/Use Cases.xlsx
@@ -2,17 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\LeagueManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\LeagueManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="8970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="8970" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Registration" sheetId="1" r:id="rId1"/>
+    <sheet name="Season" sheetId="1" r:id="rId1"/>
+    <sheet name="Register" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
   <si>
     <t>Registration System</t>
   </si>
@@ -119,13 +120,7 @@
     <t>R1</t>
   </si>
   <si>
-    <t>WF-Reg-R-1</t>
-  </si>
-  <si>
     <t>S1</t>
-  </si>
-  <si>
-    <t>WF-Reg-S-1</t>
   </si>
   <si>
     <t>User navigates to New Season Configuration
@@ -190,6 +185,81 @@
   </si>
   <si>
     <t>Season is not configured</t>
+  </si>
+  <si>
+    <t>UC.Reg.2</t>
+  </si>
+  <si>
+    <t>Register Player</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Any user including a new user</t>
+  </si>
+  <si>
+    <t>S.Season.1.0</t>
+  </si>
+  <si>
+    <t>Register a new player</t>
+  </si>
+  <si>
+    <t>As a User I want to Register a New Player so that I can receive the registration confirmation.</t>
+  </si>
+  <si>
+    <t>User navigates to New Player Registration
+User fills in required fields with valid data
+User leaves the player's last name empty
+User clicks Submit</t>
+  </si>
+  <si>
+    <t>Register a new player without the player's last name</t>
+  </si>
+  <si>
+    <t>Error: Last name cannot be blank
+Player is not registered</t>
+  </si>
+  <si>
+    <t>WF-Sea-E-1</t>
+  </si>
+  <si>
+    <t>WF-Sea-R-1</t>
+  </si>
+  <si>
+    <t>WF-Sea-S-1</t>
+  </si>
+  <si>
+    <t>User navigates to New Player Registration
+User fills in required fields with valid data
+User leaves the player's first name empty
+User clicks Submit</t>
+  </si>
+  <si>
+    <t>Error: First name cannot be blank
+Player is not registered</t>
+  </si>
+  <si>
+    <t>1.A.1</t>
+  </si>
+  <si>
+    <t>1.A.2</t>
+  </si>
+  <si>
+    <t>1.A.3</t>
+  </si>
+  <si>
+    <t>Register a new player without the player's date of birth</t>
+  </si>
+  <si>
+    <t>User navigates to New Player Registration
+User fills in required fields with valid data
+User leaves the player's date of birth empty
+User clicks Submit</t>
+  </si>
+  <si>
+    <t>Error: Date of birth cannot be blank
+Player is not registered</t>
   </si>
 </sst>
 </file>
@@ -251,7 +321,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -285,24 +374,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:N9" totalsRowShown="0" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:N9" totalsRowShown="0" dataDxfId="11">
   <autoFilter ref="A5:N9"/>
   <tableColumns count="14">
     <tableColumn id="1" name="Use Case Id"/>
     <tableColumn id="14" name="Use Case Name"/>
     <tableColumn id="13" name="Role Name"/>
-    <tableColumn id="2" name="Role Description" dataDxfId="5"/>
+    <tableColumn id="2" name="Role Description" dataDxfId="10"/>
     <tableColumn id="3" name="Story Id"/>
     <tableColumn id="4" name="StoryName"/>
-    <tableColumn id="5" name="StoryDescription" dataDxfId="4"/>
+    <tableColumn id="5" name="StoryDescription" dataDxfId="9"/>
     <tableColumn id="6" name="Scenario Id"/>
-    <tableColumn id="12" name="Scenario Description" dataDxfId="1"/>
+    <tableColumn id="12" name="Scenario Description" dataDxfId="8"/>
     <tableColumn id="11" name="Scenario UI"/>
     <tableColumn id="8" name="Result Id"/>
     <tableColumn id="10" name="Result UI"/>
-    <tableColumn id="9" name="Result Description" dataDxfId="3"/>
+    <tableColumn id="9" name="Result Description" dataDxfId="7"/>
+    <tableColumn id="15" name="Id" dataDxfId="6">
+      <calculatedColumnFormula>Table1[[#This Row],[Use Case Id]]&amp;";"&amp;Table1[[#This Row],[Story Id]]&amp;";"&amp;Table1[[#This Row],[Scenario Id]]&amp;":"&amp;Table1[[#This Row],[Result Id]]&amp;"["&amp;Table1[[#This Row],[Result UI]]&amp;"]"</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A5:N9" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A5:N9"/>
+  <tableColumns count="14">
+    <tableColumn id="1" name="Use Case Id"/>
+    <tableColumn id="14" name="Use Case Name"/>
+    <tableColumn id="13" name="Role Name"/>
+    <tableColumn id="2" name="Role Description" dataDxfId="4"/>
+    <tableColumn id="3" name="Story Id"/>
+    <tableColumn id="4" name="StoryName"/>
+    <tableColumn id="5" name="StoryDescription" dataDxfId="3"/>
+    <tableColumn id="6" name="Scenario Id"/>
+    <tableColumn id="12" name="Scenario Description" dataDxfId="2"/>
+    <tableColumn id="11" name="Scenario UI"/>
+    <tableColumn id="8" name="Result Id"/>
+    <tableColumn id="10" name="Result UI"/>
+    <tableColumn id="9" name="Result Description" dataDxfId="1"/>
     <tableColumn id="15" name="Id" dataDxfId="0">
-      <calculatedColumnFormula>Table1[[#This Row],[Use Case Id]]&amp;";"&amp;Table1[[#This Row],[Story Id]]&amp;";"&amp;Table1[[#This Row],[Scenario Id]]&amp;":"&amp;Table1[[#This Row],[Result Id]]&amp;"["&amp;Table1[[#This Row],[Result UI]]&amp;"]"</calculatedColumnFormula>
+      <calculatedColumnFormula>Table13[[#This Row],[Use Case Id]]&amp;";"&amp;Table13[[#This Row],[Story Id]]&amp;";"&amp;Table13[[#This Row],[Scenario Id]]&amp;":"&amp;Table13[[#This Row],[Result Id]]&amp;"["&amp;Table13[[#This Row],[Result UI]]&amp;"]"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -572,10 +686,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,37 +721,37 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="4" t="s">
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
         <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -654,13 +769,13 @@
         <v>18</v>
       </c>
       <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
         <v>37</v>
       </c>
-      <c r="I5" t="s">
-        <v>39</v>
-      </c>
       <c r="J5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K5" t="s">
         <v>19</v>
@@ -677,10 +792,10 @@
     </row>
     <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>41</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -689,7 +804,7 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -704,29 +819,29 @@
         <v>12</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K6" t="s">
         <v>11</v>
       </c>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="N6" s="2" t="str">
         <f>Table1[[#This Row],[Use Case Id]]&amp;";"&amp;Table1[[#This Row],[Story Id]]&amp;";"&amp;Table1[[#This Row],[Scenario Id]]&amp;":"&amp;Table1[[#This Row],[Result Id]]&amp;"["&amp;Table1[[#This Row],[Result UI]]&amp;"]"</f>
-        <v>UC.Reg.1;S.Reg.1.0;1.A:E1[WF-Reg-E-1]</v>
+        <v>UC.Reg.1;S.Season.1.0;1.A:E1[WF-Sea-E-1]</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
@@ -736,29 +851,29 @@
         <v>16</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K7" t="s">
         <v>29</v>
       </c>
       <c r="L7" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="N7" s="1" t="str">
         <f>Table1[[#This Row],[Use Case Id]]&amp;";"&amp;Table1[[#This Row],[Story Id]]&amp;";"&amp;Table1[[#This Row],[Scenario Id]]&amp;":"&amp;Table1[[#This Row],[Result Id]]&amp;"["&amp;Table1[[#This Row],[Result UI]]&amp;"]"</f>
-        <v>UC.Reg.1;S.Reg.1.0;1.B:R1[WF-Reg-R-1]</v>
+        <v>UC.Reg.1;S.Season.1.0;1.B:R1[WF-Sea-R-1]</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" t="s">
@@ -768,40 +883,281 @@
         <v>26</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L8" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N8" s="1" t="str">
         <f>Table1[[#This Row],[Use Case Id]]&amp;";"&amp;Table1[[#This Row],[Story Id]]&amp;";"&amp;Table1[[#This Row],[Scenario Id]]&amp;":"&amp;Table1[[#This Row],[Result Id]]&amp;"["&amp;Table1[[#This Row],[Result UI]]&amp;"]"</f>
-        <v>UC.Reg.1;S.Reg.1.0;1.B.1:S1[WF-Reg-S-1]</v>
+        <v>UC.Reg.1;S.Season.1.0;1.B.1:S1[WF-Sea-S-1]</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N9" s="1" t="str">
         <f>Table1[[#This Row],[Use Case Id]]&amp;";"&amp;Table1[[#This Row],[Story Id]]&amp;";"&amp;Table1[[#This Row],[Scenario Id]]&amp;":"&amp;Table1[[#This Row],[Result Id]]&amp;"["&amp;Table1[[#This Row],[Result UI]]&amp;"]"</f>
         <v>;;1.B.2:[]</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" customWidth="1"/>
+    <col min="10" max="10" width="45.140625" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="59.42578125" customWidth="1"/>
+    <col min="14" max="14" width="36" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="2" t="str">
+        <f>Table13[[#This Row],[Use Case Id]]&amp;";"&amp;Table13[[#This Row],[Story Id]]&amp;";"&amp;Table13[[#This Row],[Scenario Id]]&amp;":"&amp;Table13[[#This Row],[Result Id]]&amp;"["&amp;Table13[[#This Row],[Result UI]]&amp;"]"</f>
+        <v>UC.Reg.2;S.Reg.1.0;1.A.1:E1[WF-Reg-E-1]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="1" t="str">
+        <f>Table13[[#This Row],[Use Case Id]]&amp;";"&amp;Table13[[#This Row],[Story Id]]&amp;";"&amp;Table13[[#This Row],[Scenario Id]]&amp;":"&amp;Table13[[#This Row],[Result Id]]&amp;"["&amp;Table13[[#This Row],[Result UI]]&amp;"]"</f>
+        <v>UC.Reg.1;S.Reg.1.0;1.A.2:E1[WF-Reg-E-1]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N8" s="1" t="str">
+        <f>Table13[[#This Row],[Use Case Id]]&amp;";"&amp;Table13[[#This Row],[Story Id]]&amp;";"&amp;Table13[[#This Row],[Scenario Id]]&amp;":"&amp;Table13[[#This Row],[Result Id]]&amp;"["&amp;Table13[[#This Row],[Result UI]]&amp;"]"</f>
+        <v>UC.Reg.1;S.Reg.1.0;1.A.3:E1[WF-Reg-E-1]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1" t="str">
+        <f>Table13[[#This Row],[Use Case Id]]&amp;";"&amp;Table13[[#This Row],[Story Id]]&amp;";"&amp;Table13[[#This Row],[Scenario Id]]&amp;":"&amp;Table13[[#This Row],[Result Id]]&amp;"["&amp;Table13[[#This Row],[Result UI]]&amp;"]"</f>
+        <v>;;:[]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>